<commit_message>
fix(core): fix for xlsx number value as string
</commit_message>
<xml_diff>
--- a/modules/engine/examind-engine-process-sos/src/test/resources/com/examind/process/sos/test-flat.xlsx
+++ b/modules/engine/examind-engine-process-sos/src/test/resources/com/examind/process/sos/test-flat.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t xml:space="preserve">TIME</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">PROPERTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROPNAME</t>
   </si>
   <si>
     <t xml:space="preserve">2.1</t>
@@ -74,6 +77,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -133,16 +137,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -163,100 +171,115 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>29281.9111111111</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
         <v>29281.9111111111</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>29282.9111111111</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="F4" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
         <v>29282.9111111111</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="0" t="s">
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>29282.9111111111</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
+      <c r="F5" s="3" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>